<commit_message>
fixed travel page tiles, updated cities
</commit_message>
<xml_diff>
--- a/data/travel_cities.xlsx
+++ b/data/travel_cities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\Documents\MEDS 2022-2023\kiranfavre.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A867925-33D7-4C76-B102-C639F178DE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53257DB2-C0D0-4220-B2CA-73591FD64B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-375" yWindow="615" windowWidth="14295" windowHeight="12000" xr2:uid="{480BA5CF-8559-4837-BE6C-7BD53D43F432}"/>
+    <workbookView xWindow="1357" yWindow="1800" windowWidth="14123" windowHeight="11918" xr2:uid="{480BA5CF-8559-4837-BE6C-7BD53D43F432}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
   <si>
     <t>city</t>
   </si>
@@ -360,6 +360,21 @@
   </si>
   <si>
     <t xml:space="preserve">USA </t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>Yachats</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>Joshua Tree National Park</t>
+  </si>
+  <si>
+    <t>Bend</t>
   </si>
 </sst>
 </file>
@@ -718,15 +733,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2C686F-A71D-41A1-818F-C86D94FEA7E9}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1962,6 +1977,76 @@
         <v>-156.33189999999999</v>
       </c>
     </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89">
+        <v>39.290399999999998</v>
+      </c>
+      <c r="D89">
+        <v>-76.612200000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>109</v>
+      </c>
+      <c r="B90" t="s">
+        <v>21</v>
+      </c>
+      <c r="C90">
+        <v>44.311199999999999</v>
+      </c>
+      <c r="D90">
+        <v>-124.1048</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>110</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91">
+        <v>44.636800000000001</v>
+      </c>
+      <c r="D91">
+        <v>-125.0535</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92">
+        <v>33.873399999999997</v>
+      </c>
+      <c r="D92">
+        <v>-115.901</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93">
+        <v>44.058199999999999</v>
+      </c>
+      <c r="D93">
+        <v>-121.31529999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>